<commit_message>
Add missing results for Ed Connell
</commit_message>
<xml_diff>
--- a/data/2022-03-21/SCW Weekly Comp 2022-03-21 (Responses).xlsx
+++ b/data/2022-03-21/SCW Weekly Comp 2022-03-21 (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="174">
   <si>
     <t>Timestamp</t>
   </si>
@@ -515,6 +515,24 @@
   </si>
   <si>
     <t>6:20.59</t>
+  </si>
+  <si>
+    <t>Ed Connell</t>
+  </si>
+  <si>
+    <t>2018CONN04</t>
+  </si>
+  <si>
+    <t>3x3x3 One-Handed</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/1418360898645376/?post_id=1427023837779082&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/1418360898645376/?post_id=1422308874917245&amp;view=permalink</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/events/384201419918111/?post_id=387373082934278&amp;view=permalink</t>
   </si>
 </sst>
 </file>
@@ -2712,6 +2730,123 @@
         <v>32</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" s="2">
+        <v>44655.45653429398</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="AT43" s="3">
+        <v>35.01</v>
+      </c>
+      <c r="AU43" s="3">
+        <v>40.62</v>
+      </c>
+      <c r="AV43" s="3">
+        <v>32.24</v>
+      </c>
+      <c r="AW43" s="3">
+        <v>33.88</v>
+      </c>
+      <c r="AX43" s="3">
+        <v>46.57</v>
+      </c>
+      <c r="AY43" s="3">
+        <v>32.24</v>
+      </c>
+      <c r="AZ43" s="3">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2">
+        <v>44655.45730012732</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="O44" s="3">
+        <v>16.04</v>
+      </c>
+      <c r="P44" s="3">
+        <v>16.43</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>19.52</v>
+      </c>
+      <c r="R44" s="3">
+        <v>15.83</v>
+      </c>
+      <c r="S44" s="3">
+        <v>15.44</v>
+      </c>
+      <c r="T44" s="3">
+        <v>15.44</v>
+      </c>
+      <c r="U44" s="3">
+        <v>16.1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2">
+        <v>44655.45818696759</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="CJ45" s="3">
+        <v>33.0</v>
+      </c>
+      <c r="CK45" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="CL45" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="CM45" s="3">
+        <v>33.0</v>
+      </c>
+      <c r="CN45" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F2"/>
@@ -2755,7 +2890,10 @@
     <hyperlink r:id="rId39" ref="F40"/>
     <hyperlink r:id="rId40" ref="F41"/>
     <hyperlink r:id="rId41" ref="F42"/>
+    <hyperlink r:id="rId42" ref="F43"/>
+    <hyperlink r:id="rId43" ref="F44"/>
+    <hyperlink r:id="rId44" ref="F45"/>
   </hyperlinks>
-  <drawing r:id="rId42"/>
+  <drawing r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>